<commit_message>
Commit changes to git
</commit_message>
<xml_diff>
--- a/DataDrivenFramework_POI/TestData/Testdata - Copy.xlsx
+++ b/DataDrivenFramework_POI/TestData/Testdata - Copy.xlsx
@@ -3,25 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manda\eclipse-workspace\DataDrivenFramework_POI\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manda\git\DataDrivenFramework_POI\DataDrivenFramework_POI\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F511E23-D496-4E38-BCF9-07FA8A8AFA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C35E68-538E-45F3-A0B2-81DECC2C2701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1152" windowWidth="21600" windowHeight="11208" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
     <sheet name="Employee" sheetId="2" r:id="rId2"/>
     <sheet name="Contactdetails" sheetId="3" r:id="rId3"/>
     <sheet name="FBLogin" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="GmailLogin" sheetId="5" r:id="rId5"/>
+    <sheet name="GoogleSearch" sheetId="6" r:id="rId6"/>
+    <sheet name="BalajiLogin" sheetId="7" r:id="rId7"/>
+    <sheet name="SimpleInterest" sheetId="8" r:id="rId8"/>
+    <sheet name="CompoundInterest" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -157,28 +161,179 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>TestResults</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>mipgtestuser@gmail.com</t>
+  </si>
+  <si>
+    <t>MIPG@test</t>
+  </si>
+  <si>
+    <t>test4@gmail.com</t>
+  </si>
+  <si>
+    <t>test@4</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Searchtext</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Maven</t>
+  </si>
+  <si>
+    <t>Test NG</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>AddressLine1</t>
+  </si>
+  <si>
+    <t>AddressLine2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>PhotoIDProof</t>
+  </si>
+  <si>
+    <t>PhotoIDCard</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Katragadda</t>
+  </si>
+  <si>
+    <t>8019998710</t>
+  </si>
+  <si>
+    <t>Addresstest</t>
+  </si>
+  <si>
+    <t>Addresstest1</t>
+  </si>
+  <si>
+    <t>Kukatpally</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Driving License</t>
+  </si>
+  <si>
+    <t>K878678235</t>
+  </si>
+  <si>
+    <t>Testing@1</t>
+  </si>
+  <si>
+    <t>Mandava</t>
+  </si>
+  <si>
+    <t>8019998711</t>
+  </si>
+  <si>
+    <t>Addresstest2</t>
+  </si>
+  <si>
+    <t>Addresstest3</t>
+  </si>
+  <si>
+    <t>Ameerpet</t>
+  </si>
+  <si>
+    <t>K878678236</t>
+  </si>
+  <si>
+    <t>Testing@2</t>
+  </si>
+  <si>
+    <t>Principle</t>
+  </si>
+  <si>
+    <t>Rate of Interest</t>
+  </si>
+  <si>
+    <t>Period (Years)</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Simple Interest</t>
+  </si>
+  <si>
+    <t>Maturity Value</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Compounded Yearly</t>
+  </si>
+  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>TestResults</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Age</t>
+    <t>Test Failed</t>
+  </si>
+  <si>
+    <t>Test Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,7 +373,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -226,15 +381,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -518,112 +692,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -638,67 +854,67 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -713,44 +929,44 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -764,70 +980,62 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -847,12 +1055,543 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0BF769-AC57-48F0-AFD8-EEE2B337A4E4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="34.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7094F8F6-F960-48C3-8F6E-ADD2323B0DC4}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{94666D71-C9B0-4FD9-9F55-9B4EC8091BE4}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{D41A5661-A878-4A59-BBBF-3CF9A139DF24}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{08221203-3CF8-487B-A30B-7C79673F11ED}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{C39AD8E0-1400-42BC-A095-90F7B04B6F01}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{463AFC3F-C615-4849-B7A8-58793B36E40E}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{75467CF2-AF9E-4D7B-88D9-7168057CDB5F}"/>
+    <hyperlink ref="B5" r:id="rId8" xr:uid="{4DC8AB17-2A81-4656-894B-8961A3AC537A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01590EE-0710-4151-B5A0-BBCAC7994D9F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE2F9B2-6CC8-476F-BA00-2DE5E7F695C7}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.33203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1">
+        <v>501032</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1">
+        <v>501033</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{823FA7A9-3398-484E-9EF8-A1BF4A22ABC4}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{8EDA8477-D435-4B6D-9FF8-523688DAA75E}"/>
+    <hyperlink ref="N2" r:id="rId3" xr:uid="{3CCBAA16-CCAB-4A6F-8C4A-309CAB3A2E39}"/>
+    <hyperlink ref="L3" r:id="rId4" xr:uid="{5E4D9BEE-DE95-4E89-9478-F4592CDC369C}"/>
+    <hyperlink ref="M3" r:id="rId5" xr:uid="{25F130FC-3827-492B-AB44-EB1C931719F8}"/>
+    <hyperlink ref="N3" r:id="rId6" xr:uid="{DE7129EB-74B8-4124-BDB8-733F3E9AD9D5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36208C5E-1BFB-4EC3-9261-FACB3AEFE5C6}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>4567</v>
+      </c>
+      <c r="B3" s="1">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8352.56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="1">
+        <v>65000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>75000</v>
+      </c>
+      <c r="B5" s="5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="5">
+        <v>84000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC224C8C-6207-428E-8883-3AFC22E1221C}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2456</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2">
+        <v>3914.99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>35000</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3">
+        <v>109844.99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>50000</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4">
+        <v>60949.72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>